<commit_message>
Changed issued date and citation dates in CLRs/OLRs to 2017, also QA fixes
</commit_message>
<xml_diff>
--- a/datamares/CLR/CLR_datamares_ecosystems.xlsx
+++ b/datamares/CLR/CLR_datamares_ecosystems.xlsx
@@ -1919,9 +1919,6 @@
     <t>Scripps Institution of Oceanography</t>
   </si>
   <si>
-    <t>2016</t>
-  </si>
-  <si>
     <t>The dataMares Collection contains a selection of datasets associated with specific "stories", or topics, at http://datamares.ucsd.edu. Within the landing pages for each dataset in this collection, links to the associated stories are provided under Related Resource. Likewise, links to the datasets herein are provided on the story pages at the dataMares website. Additionally, the dataMares Projects (e.g., Fisheries, Mangroves, Proyecto Manta) are represented here as subcollections, each containing a subset of the data contained within the umbrella of the dataMares Collection.
 This collection is a work in progress. Datasets will be added as they are compiled and contributed to http://datamares.ucsd.edu.</t>
   </si>
@@ -1954,6 +1951,9 @@
   </si>
   <si>
     <t>Marine ecosystems</t>
+  </si>
+  <si>
+    <t>2017</t>
   </si>
 </sst>
 </file>
@@ -2984,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3064,7 +3064,7 @@
         <v>630</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>472</v>
@@ -3076,40 +3076,40 @@
         <v>432</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>631</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>634</v>
-      </c>
       <c r="Q2" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>